<commit_message>
Ajout Essai 3 avec un filet à poisson au lieu d'un aimant
Ajout d'une poigner
+ Modif mineurs
</commit_message>
<xml_diff>
--- a/comparaison_electro_aimant.xlsx
+++ b/comparaison_electro_aimant.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\Meca_Robot\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="17475" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -173,8 +178,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="6" formatCode="#,##0\ &quot;€&quot;_);[Red]\(#,##0\ &quot;€&quot;\)"/>
-    <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;€&quot;_);[Red]\(#,##0.00\ &quot;€&quot;\)"/>
+    <numFmt numFmtId="164" formatCode="#,##0\ &quot;€&quot;_);[Red]\(#,##0\ &quot;€&quot;\)"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;_);[Red]\(#,##0.00\ &quot;€&quot;\)"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -208,12 +213,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -232,21 +243,31 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -575,24 +596,24 @@
   <dimension ref="C3:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="21.5" customWidth="1"/>
     <col min="6" max="6" width="21.5" customWidth="1"/>
-    <col min="7" max="7" width="11.83203125" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" customWidth="1"/>
+    <col min="7" max="7" width="11.875" customWidth="1"/>
+    <col min="8" max="8" width="12.625" customWidth="1"/>
     <col min="9" max="9" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:9" ht="20">
+    <row r="3" spans="3:9" ht="21" x14ac:dyDescent="0.35">
       <c r="D3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="3:9">
+    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>2</v>
       </c>
@@ -615,7 +636,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="3:9">
+    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>1</v>
       </c>
@@ -626,7 +647,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="3:9">
+    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>7</v>
       </c>
@@ -649,7 +670,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="3:9">
+    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>16</v>
       </c>
@@ -672,30 +693,30 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="3:9">
-      <c r="C9" t="s">
+    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9" s="5">
         <v>17.5</v>
       </c>
     </row>
-    <row r="10" spans="3:9">
+    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>31</v>
       </c>
@@ -718,7 +739,7 @@
         <v>28.85</v>
       </c>
     </row>
-    <row r="11" spans="3:9">
+    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>32</v>
       </c>
@@ -741,7 +762,7 @@
         <v>16.600000000000001</v>
       </c>
     </row>
-    <row r="12" spans="3:9">
+    <row r="12" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>38</v>
       </c>
@@ -764,7 +785,7 @@
         <v>23.98</v>
       </c>
     </row>
-    <row r="13" spans="3:9">
+    <row r="13" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>40</v>
       </c>
@@ -787,7 +808,7 @@
         <v>29.67</v>
       </c>
     </row>
-    <row r="14" spans="3:9">
+    <row r="14" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>45</v>
       </c>

</xml_diff>